<commit_message>
chore: fix batch templates
</commit_message>
<xml_diff>
--- a/public/batch_record_template.xlsx
+++ b/public/batch_record_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lawrence/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8F3F308-1E79-AF48-B155-9038C76E8C59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{79B288F2-BC1A-3345-9E09-3222A7AB4877}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="880" windowWidth="41120" windowHeight="24280" xr2:uid="{F532AAA1-3791-1543-91C2-E0C6ACA55344}"/>
+    <workbookView xWindow="0" yWindow="880" windowWidth="38400" windowHeight="19740" xr2:uid="{F532AAA1-3791-1543-91C2-E0C6ACA55344}"/>
   </bookViews>
   <sheets>
     <sheet name="batch" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
   <si>
     <t>FirstName</t>
   </si>
@@ -52,9 +52,6 @@
     <t>tz@example.com</t>
   </si>
   <si>
-    <t>XXXXXX/10/1</t>
-  </si>
-  <si>
     <t>Hope</t>
   </si>
   <si>
@@ -64,24 +61,6 @@
     <t>ht@example.com</t>
   </si>
   <si>
-    <t>XXXXXX/64/1</t>
-  </si>
-  <si>
-    <t>0967XXXXXX</t>
-  </si>
-  <si>
-    <t>000XXXXXXXXXX</t>
-  </si>
-  <si>
-    <t>0965XXXXXX</t>
-  </si>
-  <si>
-    <t>0975XXXXXX</t>
-  </si>
-  <si>
-    <t>097XXXXX</t>
-  </si>
-  <si>
     <t>Gift</t>
   </si>
   <si>
@@ -89,6 +68,39 @@
   </si>
   <si>
     <t>gt@example.com</t>
+  </si>
+  <si>
+    <t>0967123456</t>
+  </si>
+  <si>
+    <t>0965123456</t>
+  </si>
+  <si>
+    <t>0951234567</t>
+  </si>
+  <si>
+    <t>334982/10/1</t>
+  </si>
+  <si>
+    <t>123456/64/1</t>
+  </si>
+  <si>
+    <t>AccountType</t>
+  </si>
+  <si>
+    <t>mobile</t>
+  </si>
+  <si>
+    <t>0975123456</t>
+  </si>
+  <si>
+    <t>bank</t>
+  </si>
+  <si>
+    <t>0972123321</t>
+  </si>
+  <si>
+    <t>1234567890123</t>
   </si>
 </sst>
 </file>
@@ -581,9 +593,11 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -940,20 +954,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{703E5390-1974-9641-A579-4DA0C0039EB5}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -963,20 +978,23 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="H1" s="2" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -986,63 +1004,72 @@
       <c r="C2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="2" t="s">
         <v>17</v>
       </c>
       <c r="E2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="3">
+        <v>10.119999999999999</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>10</v>
       </c>
-      <c r="F2" t="s">
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G3" s="3">
+        <v>100</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G2">
-        <v>20000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="D4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3">
-        <v>20000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="E4" t="s">
         <v>20</v>
       </c>
-      <c r="B4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" s="1" t="s">
+      <c r="F4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G4" s="3">
+        <v>50.54</v>
+      </c>
+      <c r="H4" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="D4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G4">
-        <v>20000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix: update and clean ups
</commit_message>
<xml_diff>
--- a/public/batch_record_template.xlsx
+++ b/public/batch_record_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lawrence/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{79B288F2-BC1A-3345-9E09-3222A7AB4877}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{CAB88A44-595F-814F-8C39-0AC31931802D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="880" windowWidth="38400" windowHeight="19740" xr2:uid="{F532AAA1-3791-1543-91C2-E0C6ACA55344}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="31">
   <si>
     <t>FirstName</t>
   </si>
@@ -101,6 +101,18 @@
   </si>
   <si>
     <t>1234567890123</t>
+  </si>
+  <si>
+    <t>Narration</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>Test again</t>
+  </si>
+  <si>
+    <t>Awesome test</t>
   </si>
 </sst>
 </file>
@@ -954,10 +966,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{703E5390-1974-9641-A579-4DA0C0039EB5}">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -968,7 +980,7 @@
     <col min="7" max="7" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -993,8 +1005,11 @@
       <c r="H1" s="2" t="s">
         <v>21</v>
       </c>
+      <c r="I1" s="2" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -1019,8 +1034,11 @@
       <c r="H2" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="I2" s="2" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -1045,8 +1063,11 @@
       <c r="H3" s="2" t="s">
         <v>24</v>
       </c>
+      <c r="I3" s="2" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -1070,6 +1091,9 @@
       </c>
       <c r="H4" s="2" t="s">
         <v>22</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>